<commit_message>
Se terminaron los scripts de QuickSort
</commit_message>
<xml_diff>
--- a/Hugo Hernan Henao/Trimestre IV/Evidencias/QuickSort/Documentos/Diagrama de Gantt.xlsx
+++ b/Hugo Hernan Henao/Trimestre IV/Evidencias/QuickSort/Documentos/Diagrama de Gantt.xlsx
@@ -339,6 +339,101 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,101 +452,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,7 +735,7 @@
   <dimension ref="B2:AC32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28:R28"/>
+      <selection activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -746,28 +746,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="34"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="32"/>
       <c r="V2" s="11"/>
       <c r="W2" s="12"/>
       <c r="X2" s="12"/>
@@ -778,26 +778,26 @@
       <c r="AC2" s="13"/>
     </row>
     <row r="3" spans="2:29" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="35"/>
       <c r="V3" s="11"/>
       <c r="W3" s="12"/>
       <c r="X3" s="12"/>
@@ -808,28 +808,28 @@
       <c r="AC3" s="13"/>
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
-      <c r="U4" s="43"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="26"/>
       <c r="V4" s="14"/>
       <c r="W4" s="15"/>
       <c r="X4" s="15"/>
@@ -840,26 +840,26 @@
       <c r="AC4" s="13"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="46"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="29"/>
       <c r="V5" s="14"/>
       <c r="W5" s="15"/>
       <c r="X5" s="15"/>
@@ -870,28 +870,28 @@
       <c r="AC5" s="13"/>
     </row>
     <row r="6" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="34"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="32"/>
       <c r="V6" s="11"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
@@ -902,26 +902,26 @@
       <c r="AC6" s="13"/>
     </row>
     <row r="7" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="38"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="40"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="35"/>
       <c r="V7" s="11"/>
       <c r="W7" s="12"/>
       <c r="X7" s="12"/>
@@ -932,28 +932,28 @@
       <c r="AC7" s="13"/>
     </row>
     <row r="8" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="48"/>
-      <c r="U8" s="49"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="37"/>
+      <c r="U8" s="38"/>
       <c r="V8" s="16"/>
       <c r="W8" s="17"/>
       <c r="X8" s="17"/>
@@ -964,26 +964,26 @@
       <c r="AC8" s="13"/>
     </row>
     <row r="9" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B9" s="50"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="51"/>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="51"/>
-      <c r="S9" s="51"/>
-      <c r="T9" s="51"/>
-      <c r="U9" s="52"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="41"/>
       <c r="V9" s="16"/>
       <c r="W9" s="17"/>
       <c r="X9" s="17"/>
@@ -994,28 +994,28 @@
       <c r="AC9" s="13"/>
     </row>
     <row r="10" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="33"/>
-      <c r="S10" s="33"/>
-      <c r="T10" s="33"/>
-      <c r="U10" s="34"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="32"/>
       <c r="V10" s="11"/>
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
@@ -1026,26 +1026,26 @@
       <c r="AC10" s="13"/>
     </row>
     <row r="11" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="40"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="35"/>
       <c r="V11" s="11"/>
       <c r="W11" s="12"/>
       <c r="X11" s="12"/>
@@ -1056,28 +1056,28 @@
       <c r="AC11" s="13"/>
     </row>
     <row r="12" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="48"/>
-      <c r="S12" s="48"/>
-      <c r="T12" s="48"/>
-      <c r="U12" s="49"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="38"/>
       <c r="V12" s="16"/>
       <c r="W12" s="17"/>
       <c r="X12" s="17"/>
@@ -1088,26 +1088,26 @@
       <c r="AC12" s="13"/>
     </row>
     <row r="13" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="51"/>
-      <c r="S13" s="51"/>
-      <c r="T13" s="51"/>
-      <c r="U13" s="52"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="U13" s="41"/>
       <c r="V13" s="16"/>
       <c r="W13" s="17"/>
       <c r="X13" s="17"/>
@@ -1118,28 +1118,28 @@
       <c r="AC13" s="13"/>
     </row>
     <row r="14" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="54"/>
-      <c r="U14" s="55"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="44"/>
       <c r="V14" s="18"/>
       <c r="W14" s="19"/>
       <c r="X14" s="19"/>
@@ -1150,26 +1150,26 @@
       <c r="AC14" s="13"/>
     </row>
     <row r="15" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="56"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="57"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="57"/>
-      <c r="R15" s="57"/>
-      <c r="S15" s="57"/>
-      <c r="T15" s="57"/>
-      <c r="U15" s="58"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="46"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="46"/>
+      <c r="Q15" s="46"/>
+      <c r="R15" s="46"/>
+      <c r="S15" s="46"/>
+      <c r="T15" s="46"/>
+      <c r="U15" s="47"/>
       <c r="V15" s="18"/>
       <c r="W15" s="19"/>
       <c r="X15" s="19"/>
@@ -1180,28 +1180,28 @@
       <c r="AC15" s="13"/>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
-      <c r="U16" s="43"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="26"/>
       <c r="V16" s="14"/>
       <c r="W16" s="15"/>
       <c r="X16" s="15"/>
@@ -1212,26 +1212,26 @@
       <c r="AC16" s="13"/>
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
-      <c r="U17" s="46"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="29"/>
       <c r="V17" s="14"/>
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
@@ -1242,30 +1242,30 @@
       <c r="AC17" s="13"/>
     </row>
     <row r="18" spans="2:29" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="22" t="s">
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="24"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="56"/>
+      <c r="P18" s="56"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="56"/>
+      <c r="S18" s="56"/>
+      <c r="T18" s="56"/>
+      <c r="U18" s="57"/>
       <c r="V18" s="20"/>
       <c r="W18" s="21"/>
       <c r="X18" s="21"/>
@@ -1276,30 +1276,30 @@
       <c r="AC18" s="13"/>
     </row>
     <row r="19" spans="2:29" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="35"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="25" t="s">
+      <c r="B19" s="49"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="25" t="s">
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="R19" s="26"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="26"/>
-      <c r="U19" s="27"/>
+      <c r="R19" s="59"/>
+      <c r="S19" s="59"/>
+      <c r="T19" s="59"/>
+      <c r="U19" s="60"/>
       <c r="V19" s="10"/>
       <c r="W19" s="9"/>
       <c r="X19" s="9"/>
@@ -1309,14 +1309,14 @@
       <c r="AB19" s="9"/>
     </row>
     <row r="20" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="40"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="3">
         <v>17</v>
       </c>
@@ -1362,16 +1362,16 @@
       <c r="AB20" s="9"/>
     </row>
     <row r="21" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
       <c r="J21" s="4"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1393,16 +1393,16 @@
       <c r="AB21" s="9"/>
     </row>
     <row r="22" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
       <c r="J22" s="4"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -1424,16 +1424,16 @@
       <c r="AB22" s="9"/>
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="30"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="54"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -1455,16 +1455,16 @@
       <c r="AB23" s="9"/>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="5"/>
@@ -1486,22 +1486,22 @@
       <c r="AB24" s="9"/>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="30"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="54"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="59"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="22"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
@@ -1517,22 +1517,22 @@
       <c r="AB25" s="9"/>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="60"/>
-      <c r="N26" s="60"/>
-      <c r="O26" s="60"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="2"/>
@@ -1548,22 +1548,22 @@
       <c r="AB26" s="9"/>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="60"/>
-      <c r="L27" s="60"/>
-      <c r="M27" s="60"/>
-      <c r="N27" s="60"/>
-      <c r="O27" s="60"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="2"/>
@@ -1579,26 +1579,26 @@
       <c r="AB27" s="9"/>
     </row>
     <row r="28" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="60"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="60"/>
-      <c r="O28" s="60"/>
-      <c r="P28" s="60"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
-      <c r="S28" s="2"/>
+      <c r="S28" s="4"/>
       <c r="T28" s="2"/>
       <c r="U28" s="7"/>
       <c r="V28" s="10"/>
@@ -1610,16 +1610,16 @@
       <c r="AB28" s="9"/>
     </row>
     <row r="29" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="48"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
@@ -1628,8 +1628,8 @@
       <c r="O29" s="2"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="2"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="4"/>
       <c r="T29" s="2"/>
       <c r="U29" s="7"/>
       <c r="V29" s="10"/>
@@ -1641,16 +1641,16 @@
       <c r="AB29" s="9"/>
     </row>
     <row r="30" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -1659,8 +1659,8 @@
       <c r="O30" s="2"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="2"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="4"/>
       <c r="T30" s="2"/>
       <c r="U30" s="7"/>
       <c r="V30" s="10"/>
@@ -1672,16 +1672,16 @@
       <c r="AB30" s="9"/>
     </row>
     <row r="31" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
@@ -1690,7 +1690,7 @@
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="5"/>
-      <c r="R31" s="4"/>
+      <c r="R31" s="5"/>
       <c r="S31" s="4"/>
       <c r="T31" s="4"/>
       <c r="U31" s="8"/>
@@ -1703,16 +1703,16 @@
       <c r="AB31" s="9"/>
     </row>
     <row r="32" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -1735,14 +1735,11 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B16:U17"/>
-    <mergeCell ref="B2:U3"/>
-    <mergeCell ref="B4:U5"/>
-    <mergeCell ref="B6:U7"/>
-    <mergeCell ref="B8:U9"/>
-    <mergeCell ref="B10:U11"/>
-    <mergeCell ref="B12:U13"/>
-    <mergeCell ref="B14:U15"/>
+    <mergeCell ref="J18:U18"/>
+    <mergeCell ref="J19:P19"/>
+    <mergeCell ref="Q19:U19"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B29:I29"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="B31:I31"/>
     <mergeCell ref="B32:I32"/>
@@ -1754,11 +1751,14 @@
     <mergeCell ref="B28:I28"/>
     <mergeCell ref="B25:I25"/>
     <mergeCell ref="B27:I27"/>
-    <mergeCell ref="J18:U18"/>
-    <mergeCell ref="J19:P19"/>
-    <mergeCell ref="Q19:U19"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B16:U17"/>
+    <mergeCell ref="B2:U3"/>
+    <mergeCell ref="B4:U5"/>
+    <mergeCell ref="B6:U7"/>
+    <mergeCell ref="B8:U9"/>
+    <mergeCell ref="B10:U11"/>
+    <mergeCell ref="B12:U13"/>
+    <mergeCell ref="B14:U15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>